<commit_message>
separate payment status and delivery status
</commit_message>
<xml_diff>
--- a/purchase_data.xlsx
+++ b/purchase_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AG3"/>
+  <dimension ref="A1:R2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -471,132 +471,57 @@
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>Status</t>
+          <t>입고상태</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
+          <t>지급상태</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
           <t>견적서경로</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>품목명</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>모델명</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>Description</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>수량</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>단가</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>공급가액</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>세액</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>합계금액</t>
-        </is>
-      </c>
-      <c r="R1" s="1" t="inlineStr">
-        <is>
-          <t>환율</t>
-        </is>
-      </c>
-      <c r="S1" s="1" t="inlineStr">
-        <is>
-          <t>주문요청사항</t>
-        </is>
-      </c>
-      <c r="T1" s="1" t="inlineStr">
-        <is>
-          <t>견적일</t>
-        </is>
-      </c>
-      <c r="U1" s="1" t="inlineStr">
-        <is>
-          <t>발주서번호</t>
-        </is>
-      </c>
-      <c r="V1" s="1" t="inlineStr">
-        <is>
-          <t>발주서경로</t>
-        </is>
-      </c>
-      <c r="W1" s="1" t="inlineStr">
-        <is>
-          <t>입고예정일</t>
-        </is>
-      </c>
-      <c r="X1" s="1" t="inlineStr">
-        <is>
-          <t>입고일</t>
-        </is>
-      </c>
-      <c r="Y1" s="1" t="inlineStr">
-        <is>
-          <t>운송방법</t>
-        </is>
-      </c>
-      <c r="Z1" s="1" t="inlineStr">
-        <is>
-          <t>송장번호</t>
-        </is>
-      </c>
-      <c r="AA1" s="1" t="inlineStr">
-        <is>
-          <t>운송장경로</t>
-        </is>
-      </c>
-      <c r="AB1" s="1" t="inlineStr">
-        <is>
-          <t>미지급액</t>
-        </is>
-      </c>
-      <c r="AC1" s="1" t="inlineStr">
-        <is>
-          <t>지급액</t>
-        </is>
-      </c>
-      <c r="AD1" s="1" t="inlineStr">
-        <is>
-          <t>지급일</t>
-        </is>
-      </c>
-      <c r="AE1" s="1" t="inlineStr">
-        <is>
-          <t>세금계산서발행일</t>
-        </is>
-      </c>
-      <c r="AF1" s="1" t="inlineStr">
-        <is>
-          <t>계산서번호</t>
-        </is>
-      </c>
-      <c r="AG1" s="1" t="inlineStr">
-        <is>
-          <t>수입신고번호</t>
         </is>
       </c>
     </row>
@@ -626,155 +551,57 @@
           <t>KRW</t>
         </is>
       </c>
-      <c r="F2" t="n">
-        <v>10</v>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
+          <t>ㅁㄴㅇㄹㄴㅁㅇㄹㄷㅈㄹ</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>미입고</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>미지급</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr"/>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>ㅁㄴㅇㄻㄴㅇ</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>ㄻㄴㅇㄹㅁㄴㅇㄻㄴㅇㄹ</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
           <t>ㅁㄴㅇㄻㄴㅇㄹ</t>
         </is>
       </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>발주</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr"/>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>ㅁㄴㅇㄹ</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>ㅁㄴㅇㄹ</t>
-        </is>
-      </c>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>ㅁㄴㅇㄹ</t>
-        </is>
-      </c>
-      <c r="M2" t="n">
+      <c r="N2" t="n">
         <v>1</v>
       </c>
-      <c r="N2" t="n">
+      <c r="O2" t="n">
+        <v>10000</v>
+      </c>
+      <c r="P2" t="n">
+        <v>10000</v>
+      </c>
+      <c r="Q2" t="n">
         <v>1000</v>
       </c>
-      <c r="O2" t="n">
-        <v>1000</v>
-      </c>
-      <c r="P2" t="n">
-        <v>100</v>
-      </c>
-      <c r="Q2" t="n">
-        <v>1100</v>
-      </c>
-      <c r="R2" t="inlineStr"/>
-      <c r="S2" t="inlineStr"/>
-      <c r="T2" t="inlineStr"/>
-      <c r="U2" t="inlineStr"/>
-      <c r="V2" t="inlineStr"/>
-      <c r="W2" t="inlineStr"/>
-      <c r="X2" t="inlineStr"/>
-      <c r="Y2" t="inlineStr"/>
-      <c r="Z2" t="inlineStr"/>
-      <c r="AA2" t="inlineStr"/>
-      <c r="AB2" t="inlineStr"/>
-      <c r="AC2" t="inlineStr"/>
-      <c r="AD2" t="inlineStr"/>
-      <c r="AE2" t="inlineStr"/>
-      <c r="AF2" t="inlineStr"/>
-      <c r="AG2" t="inlineStr"/>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>PU-251209-002</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>2025-12-09</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>내수</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>콕스</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>KRW</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>ㅁㄴㅇㄻㄴㅇㄹ</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>발주</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr"/>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>ㅁㄴㅇㄹ</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>ㅁㄴㅇㄹ</t>
-        </is>
-      </c>
-      <c r="L3" t="inlineStr">
-        <is>
-          <t>ㅁㄴㅇㄹ</t>
-        </is>
-      </c>
-      <c r="M3" t="n">
-        <v>1</v>
-      </c>
-      <c r="N3" t="n">
-        <v>1000</v>
-      </c>
-      <c r="O3" t="n">
-        <v>1000</v>
-      </c>
-      <c r="P3" t="n">
-        <v>100</v>
-      </c>
-      <c r="Q3" t="n">
-        <v>1100</v>
-      </c>
-      <c r="R3" t="inlineStr"/>
-      <c r="S3" t="inlineStr"/>
-      <c r="T3" t="inlineStr"/>
-      <c r="U3" t="inlineStr"/>
-      <c r="V3" t="inlineStr"/>
-      <c r="W3" t="inlineStr"/>
-      <c r="X3" t="inlineStr"/>
-      <c r="Y3" t="inlineStr"/>
-      <c r="Z3" t="inlineStr"/>
-      <c r="AA3" t="inlineStr"/>
-      <c r="AB3" t="inlineStr"/>
-      <c r="AC3" t="inlineStr"/>
-      <c r="AD3" t="inlineStr"/>
-      <c r="AE3" t="inlineStr"/>
-      <c r="AF3" t="inlineStr"/>
-      <c r="AG3" t="inlineStr"/>
+      <c r="R2" t="n">
+        <v>11000</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>